<commit_message>
Clarify which verified primes were used
</commit_message>
<xml_diff>
--- a/v1-data/results.xlsx
+++ b/v1-data/results.xlsx
@@ -209,13 +209,13 @@
     <t>More Cache advantage</t>
   </si>
   <si>
-    <t>Small Validated Riesel primes</t>
+    <t>Small Validated Riesel primes &gt; 1001 and n &lt; 1000</t>
   </si>
   <si>
-    <t>Large Validated Riesel primes</t>
+    <t>Large Validated Riesel primes n &gt;= 1000</t>
   </si>
   <si>
-    <t>All Validated Riesel primes</t>
+    <t>All Validated Riesel primes &gt; 1001</t>
   </si>
   <si>
     <t>Exceptions to the v(1) search tables</t>

</xml_diff>

<commit_message>
Added info on 4 candidates with 1st v(1) > 81
</commit_message>
<xml_diff>
--- a/v1-data/results.xlsx
+++ b/v1-data/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
   <si>
     <t>Case: h = 0 mod 3</t>
   </si>
@@ -227,7 +227,19 @@
     <t>n</t>
   </si>
   <si>
-    <t>first v(1)</t>
+    <t>first 3 v(1)</t>
+  </si>
+  <si>
+    <t>77, 87, 95</t>
+  </si>
+  <si>
+    <t>99, 107. 129</t>
+  </si>
+  <si>
+    <t>77. 87, 99</t>
+  </si>
+  <si>
+    <t>99, 101, 111</t>
   </si>
 </sst>
 </file>
@@ -2620,7 +2632,7 @@
     <xf numFmtId="0" fontId="0" borderId="103" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="104" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="104" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="105" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2632,7 +2644,7 @@
     <xf numFmtId="0" fontId="0" borderId="107" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="108" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="108" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="109" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2641,7 +2653,7 @@
     <xf numFmtId="0" fontId="0" borderId="110" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="111" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="111" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6575,8 +6587,8 @@
       <c r="B46" s="210">
         <v>1392575</v>
       </c>
-      <c r="C46" s="211">
-        <v>77</v>
+      <c r="C46" t="s" s="211">
+        <v>44</v>
       </c>
       <c r="D46" s="212"/>
       <c r="E46" s="113"/>
@@ -6611,8 +6623,8 @@
       <c r="B47" s="214">
         <v>3727349</v>
       </c>
-      <c r="C47" s="215">
-        <v>99</v>
+      <c r="C47" t="s" s="215">
+        <v>45</v>
       </c>
       <c r="D47" s="212"/>
       <c r="E47" s="113"/>
@@ -6647,8 +6659,8 @@
       <c r="B48" s="214">
         <v>5718540</v>
       </c>
-      <c r="C48" s="215">
-        <v>77</v>
+      <c r="C48" t="s" s="215">
+        <v>46</v>
       </c>
       <c r="D48" s="212"/>
       <c r="E48" s="113"/>
@@ -6683,8 +6695,8 @@
       <c r="B49" s="217">
         <v>132175294</v>
       </c>
-      <c r="C49" s="218">
-        <v>99</v>
+      <c r="C49" t="s" s="218">
+        <v>47</v>
       </c>
       <c r="D49" s="212"/>
       <c r="E49" s="113"/>

</xml_diff>